<commit_message>
Article: Lembar Kerja: Rancang Form
</commit_message>
<xml_diff>
--- a/assets/posts/lembarkerja/2018/09/05-faktur.xlsx
+++ b/assets/posts/lembarkerja/2018/09/05-faktur.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Mentah" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,15 +14,15 @@
     <sheet name="Form" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">Form!$A$1:$L$13</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">Kosong!$A$1:$L$13</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Mentah!$B$2:$V$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">Ringkas!$A$3:$L$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Mentah!$A$2:$V$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">Mentah!$B$2:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0" vbProcedure="false">Ringkas!$B$2:$L$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0" vbProcedure="false">Ringkas!$B$2:$J$6</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">Form!$B$1:$K$33</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">Kosong!$A$1:$L$13</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Mentah!$A$2:$V$8</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">Ringkas!$A$3:$L$8</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Mentah!$B$2:$V$8</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Mentah!$B$2:$K$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">Ringkas!$B$2:$L$8</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0" vbProcedure="false">Ringkas!$B$2:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">Form!$A$1:$L$13</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -250,19 +250,21 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="\ * #,##0\ ;\-* #,##0\ ;\ * &quot;- &quot;;\ @\ "/>
-    <numFmt numFmtId="166" formatCode="\ * #,##0.00\ ;\ * \(#,##0.00\);\ * \-#\ ;\ @\ "/>
-    <numFmt numFmtId="167" formatCode="dd/mm/yy"/>
-    <numFmt numFmtId="168" formatCode="#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="* #,##0\ ;\-* #,##0\ ;* &quot;- &quot;;@\ "/>
+    <numFmt numFmtId="166" formatCode="* #,##0.00\ ;* \(#,##0.00\);* \-#\ ;@\ "/>
+    <numFmt numFmtId="167" formatCode="General"/>
+    <numFmt numFmtId="168" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="169" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -292,6 +294,7 @@
       <color rgb="FF000000"/>
       <name val="Century Gothic"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -299,19 +302,37 @@
       <color rgb="FF000000"/>
       <name val="Century Gothic"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -319,6 +340,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -326,12 +348,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -461,7 +485,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="68">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -482,32 +506,48 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -530,39 +570,67 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="3" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="3" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -570,119 +638,123 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -765,16 +837,15 @@
     <tabColor rgb="FFBBDEFB"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V7"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="90" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A3:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="4.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="4.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="26.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="2" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.71"/>
@@ -790,12 +861,12 @@
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0"/>
+      <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="0"/>
-      <c r="E1" s="0"/>
-      <c r="F1" s="0"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -803,12 +874,12 @@
       <c r="K1" s="3"/>
       <c r="L1" s="4"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="0"/>
+      <c r="N1" s="1"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
-      <c r="S1" s="0"/>
+      <c r="S1" s="1"/>
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
       <c r="V1" s="1"/>
@@ -835,247 +906,303 @@
       <c r="T2" s="9"/>
       <c r="U2" s="9"/>
     </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="13"/>
+      <c r="U3" s="13"/>
+      <c r="V3" s="5"/>
+    </row>
     <row r="4" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="12" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="K4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="16" t="s">
+      <c r="L4" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="13" t="s">
+      <c r="M4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="12" t="s">
+      <c r="N4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="O4" s="13" t="s">
+      <c r="O4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="12" t="s">
+      <c r="P4" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="13" t="s">
+      <c r="Q4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="R4" s="12" t="s">
+      <c r="R4" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="S4" s="13" t="s">
+      <c r="S4" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="T4" s="12" t="s">
+      <c r="T4" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="U4" s="13" t="s">
+      <c r="U4" s="17" t="s">
         <v>19</v>
       </c>
+      <c r="V4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="17" t="n">
+      <c r="A5" s="5"/>
+      <c r="B5" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="19" t="n">
+      <c r="G5" s="23" t="n">
         <v>1</v>
       </c>
-      <c r="H5" s="19" t="n">
+      <c r="H5" s="23" t="n">
         <v>2018</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="I5" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="20" t="n">
+      <c r="J5" s="24" t="n">
         <v>12000000</v>
       </c>
-      <c r="K5" s="20" t="n">
+      <c r="K5" s="24" t="n">
         <v>1200000</v>
       </c>
-      <c r="L5" s="19" t="n">
+      <c r="L5" s="23" t="n">
         <v>0</v>
       </c>
-      <c r="M5" s="19" t="s">
+      <c r="M5" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="N5" s="18" t="s">
+      <c r="N5" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="O5" s="19" t="s">
+      <c r="O5" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="P5" s="19" t="s">
+      <c r="P5" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="Q5" s="18" t="s">
+      <c r="Q5" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="R5" s="19" t="s">
+      <c r="R5" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="S5" s="18" t="s">
+      <c r="S5" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="T5" s="19" t="s">
+      <c r="T5" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="U5" s="18"/>
+      <c r="U5" s="22"/>
+      <c r="V5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="17" t="n">
+      <c r="A6" s="5"/>
+      <c r="B6" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="19" t="n">
+      <c r="G6" s="23" t="n">
         <v>1</v>
       </c>
-      <c r="H6" s="19" t="n">
+      <c r="H6" s="23" t="n">
         <v>2018</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="I6" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="J6" s="20" t="n">
+      <c r="J6" s="24" t="n">
         <v>13000000</v>
       </c>
-      <c r="K6" s="20" t="n">
+      <c r="K6" s="24" t="n">
         <v>1300000</v>
       </c>
-      <c r="L6" s="19" t="n">
+      <c r="L6" s="23" t="n">
         <v>0</v>
       </c>
-      <c r="M6" s="19" t="s">
+      <c r="M6" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="N6" s="18" t="s">
+      <c r="N6" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="O6" s="19" t="s">
+      <c r="O6" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="P6" s="19" t="s">
+      <c r="P6" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="Q6" s="18" t="s">
+      <c r="Q6" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="R6" s="19" t="s">
+      <c r="R6" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="S6" s="18" t="s">
+      <c r="S6" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="T6" s="19" t="s">
+      <c r="T6" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="U6" s="18"/>
+      <c r="U6" s="22"/>
+      <c r="V6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="17" t="n">
+      <c r="A7" s="5"/>
+      <c r="B7" s="21" t="n">
         <v>3</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="19" t="n">
+      <c r="G7" s="23" t="n">
         <v>1</v>
       </c>
-      <c r="H7" s="19" t="n">
+      <c r="H7" s="23" t="n">
         <v>2018</v>
       </c>
-      <c r="I7" s="19" t="s">
+      <c r="I7" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="20" t="n">
+      <c r="J7" s="24" t="n">
         <v>30300000</v>
       </c>
-      <c r="K7" s="20" t="n">
+      <c r="K7" s="24" t="n">
         <v>3030000</v>
       </c>
-      <c r="L7" s="19" t="n">
+      <c r="L7" s="23" t="n">
         <v>0</v>
       </c>
-      <c r="M7" s="19" t="s">
+      <c r="M7" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="N7" s="18" t="s">
+      <c r="N7" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="O7" s="19" t="s">
+      <c r="O7" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="P7" s="19" t="s">
+      <c r="P7" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="Q7" s="18" t="s">
+      <c r="Q7" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="R7" s="19" t="s">
+      <c r="R7" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="S7" s="18" t="s">
+      <c r="S7" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="T7" s="19" t="s">
+      <c r="T7" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="U7" s="18"/>
+      <c r="U7" s="22"/>
+      <c r="V7" s="5"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1096,21 +1223,20 @@
   </sheetPr>
   <dimension ref="B2:K7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="90" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="4.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="4.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="26.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="2" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="3" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="4" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="4.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16376" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16376" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1126,156 +1252,156 @@
       <c r="K2" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="I4" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="21" t="s">
+      <c r="K4" s="29" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="17" t="n">
+      <c r="B5" s="30" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="18" t="str">
+      <c r="C5" s="31" t="str">
         <f aca="false">Mentah!C5</f>
         <v>PT. Teliti Telaten Tekun</v>
       </c>
-      <c r="D5" s="18" t="str">
+      <c r="D5" s="31" t="str">
         <f aca="false">Mentah!D5</f>
         <v>08.144.351.8-011.000</v>
       </c>
-      <c r="E5" s="18" t="str">
+      <c r="E5" s="31" t="str">
         <f aca="false">Mentah!E5</f>
         <v>010.004-18.31234567</v>
       </c>
-      <c r="F5" s="19" t="n">
+      <c r="F5" s="32" t="n">
         <f aca="false">Mentah!G5</f>
         <v>1</v>
       </c>
-      <c r="G5" s="19" t="n">
+      <c r="G5" s="32" t="n">
         <f aca="false">Mentah!H5</f>
         <v>2018</v>
       </c>
-      <c r="H5" s="19" t="str">
+      <c r="H5" s="32" t="str">
         <f aca="false">Mentah!I5</f>
         <v>Normal</v>
       </c>
-      <c r="I5" s="20" t="n">
+      <c r="I5" s="33" t="n">
         <f aca="false">Mentah!J5</f>
         <v>12000000</v>
       </c>
-      <c r="J5" s="20" t="n">
+      <c r="J5" s="33" t="n">
         <f aca="false">Mentah!K5</f>
         <v>1200000</v>
       </c>
-      <c r="K5" s="19" t="n">
+      <c r="K5" s="32" t="n">
         <f aca="false">Mentah!L5</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="17" t="n">
+      <c r="B6" s="30" t="n">
         <v>2</v>
       </c>
-      <c r="C6" s="18" t="str">
+      <c r="C6" s="31" t="str">
         <f aca="false">Mentah!C6</f>
         <v>Badan Penerbitan Sesuatu Jawa Barat</v>
       </c>
-      <c r="D6" s="18" t="str">
+      <c r="D6" s="31" t="str">
         <f aca="false">Mentah!D6</f>
         <v>03.114.215.4-271.000</v>
       </c>
-      <c r="E6" s="18" t="str">
+      <c r="E6" s="31" t="str">
         <f aca="false">Mentah!E6</f>
         <v>021.004-18.31234568</v>
       </c>
-      <c r="F6" s="19" t="n">
+      <c r="F6" s="32" t="n">
         <f aca="false">Mentah!G6</f>
         <v>1</v>
       </c>
-      <c r="G6" s="19" t="n">
+      <c r="G6" s="32" t="n">
         <f aca="false">Mentah!H6</f>
         <v>2018</v>
       </c>
-      <c r="H6" s="19" t="str">
+      <c r="H6" s="32" t="str">
         <f aca="false">Mentah!I6</f>
         <v>Batal</v>
       </c>
-      <c r="I6" s="20" t="n">
+      <c r="I6" s="33" t="n">
         <f aca="false">Mentah!J6</f>
         <v>13000000</v>
       </c>
-      <c r="J6" s="20" t="n">
+      <c r="J6" s="33" t="n">
         <f aca="false">Mentah!K6</f>
         <v>1300000</v>
       </c>
-      <c r="K6" s="19" t="n">
+      <c r="K6" s="32" t="n">
         <f aca="false">Mentah!L6</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="17" t="n">
+      <c r="B7" s="30" t="n">
         <v>3</v>
       </c>
-      <c r="C7" s="18" t="str">
+      <c r="C7" s="31" t="str">
         <f aca="false">Mentah!C7</f>
         <v>PT. Kucing Oren Lucu</v>
       </c>
-      <c r="D7" s="18" t="str">
+      <c r="D7" s="31" t="str">
         <f aca="false">Mentah!D7</f>
         <v>02.444.192.6-721.000</v>
       </c>
-      <c r="E7" s="18" t="str">
+      <c r="E7" s="31" t="str">
         <f aca="false">Mentah!E7</f>
         <v>030.004-18.31234569</v>
       </c>
-      <c r="F7" s="19" t="n">
+      <c r="F7" s="32" t="n">
         <f aca="false">Mentah!G7</f>
         <v>1</v>
       </c>
-      <c r="G7" s="19" t="n">
+      <c r="G7" s="32" t="n">
         <f aca="false">Mentah!H7</f>
         <v>2018</v>
       </c>
-      <c r="H7" s="19" t="str">
+      <c r="H7" s="32" t="str">
         <f aca="false">Mentah!I7</f>
         <v>Normal</v>
       </c>
-      <c r="I7" s="20" t="n">
+      <c r="I7" s="33" t="n">
         <f aca="false">Mentah!J7</f>
         <v>30300000</v>
       </c>
-      <c r="J7" s="20" t="n">
+      <c r="J7" s="33" t="n">
         <f aca="false">Mentah!K7</f>
         <v>3030000</v>
       </c>
-      <c r="K7" s="19" t="n">
+      <c r="K7" s="32" t="n">
         <f aca="false">Mentah!L7</f>
         <v>0</v>
       </c>
@@ -1299,8 +1425,8 @@
   </sheetPr>
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N42" activeCellId="0" sqref="N42"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="100" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N42" activeCellId="1" sqref="A3:L8 N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1321,319 +1447,319 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="21.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="21.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="13.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="23"/>
+      <c r="A1" s="34"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="35"/>
     </row>
     <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22"/>
-      <c r="B2" s="24" t="s">
+      <c r="A2" s="34"/>
+      <c r="B2" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="23"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="35"/>
       <c r="M2" s="1"/>
       <c r="R2" s="2"/>
     </row>
-    <row r="3" s="28" customFormat="true" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="23"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="S3" s="29"/>
-      <c r="T3" s="29"/>
-      <c r="XFB3" s="0"/>
-      <c r="XFC3" s="0"/>
-      <c r="XFD3" s="0"/>
-    </row>
-    <row r="4" s="28" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="22"/>
-      <c r="B4" s="30" t="s">
+    <row r="3" s="40" customFormat="true" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="35"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="41"/>
+      <c r="Q3" s="41"/>
+      <c r="S3" s="41"/>
+      <c r="T3" s="41"/>
+      <c r="XFB3" s="1"/>
+      <c r="XFC3" s="1"/>
+      <c r="XFD3" s="1"/>
+    </row>
+    <row r="4" s="40" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="34"/>
+      <c r="B4" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="32" t="s">
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="33" t="s">
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="23"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29"/>
-      <c r="S4" s="29"/>
-      <c r="T4" s="29"/>
-      <c r="XFB4" s="0"/>
-      <c r="XFC4" s="0"/>
-      <c r="XFD4" s="0"/>
-    </row>
-    <row r="5" s="28" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35" t="s">
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="35"/>
+      <c r="N4" s="41"/>
+      <c r="O4" s="41"/>
+      <c r="P4" s="41"/>
+      <c r="Q4" s="41"/>
+      <c r="S4" s="41"/>
+      <c r="T4" s="41"/>
+      <c r="XFB4" s="1"/>
+      <c r="XFC4" s="1"/>
+      <c r="XFD4" s="1"/>
+    </row>
+    <row r="5" s="40" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="34"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="36"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="23"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="S5" s="29"/>
-      <c r="T5" s="29"/>
-      <c r="XFB5" s="0"/>
-      <c r="XFC5" s="0"/>
-      <c r="XFD5" s="0"/>
-    </row>
-    <row r="6" s="28" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="22"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="39" t="s">
+      <c r="E5" s="48"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="35"/>
+      <c r="N5" s="41"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="41"/>
+      <c r="Q5" s="41"/>
+      <c r="S5" s="41"/>
+      <c r="T5" s="41"/>
+      <c r="XFB5" s="1"/>
+      <c r="XFC5" s="1"/>
+      <c r="XFD5" s="1"/>
+    </row>
+    <row r="6" s="40" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="34"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="39" t="s">
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="G6" s="41"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
-      <c r="L6" s="23"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="S6" s="29"/>
-      <c r="T6" s="29"/>
-      <c r="XFB6" s="0"/>
-      <c r="XFC6" s="0"/>
-      <c r="XFD6" s="0"/>
-    </row>
-    <row r="7" s="28" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="22"/>
-      <c r="B7" s="44"/>
-      <c r="C7" s="39" t="s">
+      <c r="G6" s="53"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="35"/>
+      <c r="N6" s="41"/>
+      <c r="O6" s="41"/>
+      <c r="P6" s="41"/>
+      <c r="Q6" s="41"/>
+      <c r="S6" s="41"/>
+      <c r="T6" s="41"/>
+      <c r="XFB6" s="1"/>
+      <c r="XFC6" s="1"/>
+      <c r="XFD6" s="1"/>
+    </row>
+    <row r="7" s="40" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="34"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="39" t="s">
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="G7" s="45"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39" t="s">
+      <c r="G7" s="57"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="46"/>
-      <c r="K7" s="47"/>
-      <c r="L7" s="48"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29"/>
-      <c r="S7" s="29"/>
-      <c r="T7" s="29"/>
-      <c r="XFB7" s="0"/>
-      <c r="XFC7" s="0"/>
-      <c r="XFD7" s="0"/>
-    </row>
-    <row r="8" s="28" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="22"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="39" t="s">
+      <c r="J7" s="58"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="60"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="41"/>
+      <c r="P7" s="41"/>
+      <c r="Q7" s="41"/>
+      <c r="S7" s="41"/>
+      <c r="T7" s="41"/>
+      <c r="XFB7" s="1"/>
+      <c r="XFC7" s="1"/>
+      <c r="XFD7" s="1"/>
+    </row>
+    <row r="8" s="40" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="34"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="39" t="s">
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="G8" s="45"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="39" t="s">
+      <c r="G8" s="57"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="J8" s="46"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="49"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
-      <c r="S8" s="29"/>
-      <c r="T8" s="29"/>
-      <c r="XFB8" s="0"/>
-      <c r="XFC8" s="0"/>
-      <c r="XFD8" s="0"/>
-    </row>
-    <row r="9" s="28" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="22"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="39" t="s">
+      <c r="J8" s="58"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="61"/>
+      <c r="N8" s="41"/>
+      <c r="O8" s="41"/>
+      <c r="P8" s="41"/>
+      <c r="Q8" s="41"/>
+      <c r="S8" s="41"/>
+      <c r="T8" s="41"/>
+      <c r="XFB8" s="1"/>
+      <c r="XFC8" s="1"/>
+      <c r="XFD8" s="1"/>
+    </row>
+    <row r="9" s="40" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="34"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39" t="s">
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="46"/>
-      <c r="K9" s="47"/>
-      <c r="L9" s="49"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-      <c r="S9" s="29"/>
-      <c r="T9" s="29"/>
-      <c r="XFB9" s="0"/>
-      <c r="XFC9" s="0"/>
-      <c r="XFD9" s="0"/>
-    </row>
-    <row r="10" s="28" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="22"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="39" t="s">
+      <c r="J9" s="58"/>
+      <c r="K9" s="59"/>
+      <c r="L9" s="61"/>
+      <c r="N9" s="41"/>
+      <c r="O9" s="41"/>
+      <c r="P9" s="41"/>
+      <c r="Q9" s="41"/>
+      <c r="S9" s="41"/>
+      <c r="T9" s="41"/>
+      <c r="XFB9" s="1"/>
+      <c r="XFC9" s="1"/>
+      <c r="XFD9" s="1"/>
+    </row>
+    <row r="10" s="40" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="34"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="39" t="s">
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="50"/>
-      <c r="L10" s="23"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="29"/>
-      <c r="S10" s="29"/>
-      <c r="T10" s="29"/>
-      <c r="XFB10" s="0"/>
-      <c r="XFC10" s="0"/>
-      <c r="XFD10" s="0"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="62"/>
+      <c r="L10" s="35"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="41"/>
+      <c r="P10" s="41"/>
+      <c r="Q10" s="41"/>
+      <c r="S10" s="41"/>
+      <c r="T10" s="41"/>
+      <c r="XFB10" s="1"/>
+      <c r="XFC10" s="1"/>
+      <c r="XFD10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="22"/>
-      <c r="B11" s="44"/>
-      <c r="C11" s="39" t="s">
+      <c r="A11" s="34"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="51" t="s">
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="G11" s="51"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="50"/>
-      <c r="L11" s="23"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="62"/>
+      <c r="L11" s="35"/>
     </row>
     <row r="12" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="22"/>
-      <c r="B12" s="52"/>
-      <c r="C12" s="53" t="s">
+      <c r="A12" s="34"/>
+      <c r="B12" s="64"/>
+      <c r="C12" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="53" t="s">
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="54"/>
-      <c r="J12" s="54"/>
-      <c r="K12" s="55"/>
-      <c r="L12" s="23"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="65"/>
+      <c r="I12" s="66"/>
+      <c r="J12" s="66"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="35"/>
       <c r="M12" s="1"/>
       <c r="R12" s="2"/>
     </row>
-    <row r="13" s="28" customFormat="true" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="23"/>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="29"/>
-      <c r="S13" s="29"/>
-      <c r="T13" s="29"/>
-      <c r="XFB13" s="0"/>
-      <c r="XFC13" s="0"/>
-      <c r="XFD13" s="0"/>
+    <row r="13" s="40" customFormat="true" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="35"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="41"/>
+      <c r="S13" s="41"/>
+      <c r="T13" s="41"/>
+      <c r="XFB13" s="1"/>
+      <c r="XFC13" s="1"/>
+      <c r="XFD13" s="1"/>
     </row>
     <row r="1048502" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048503" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1750,8 +1876,8 @@
   </sheetPr>
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M37" activeCellId="0" sqref="M37"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="100" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="1" sqref="A3:L8 D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1772,757 +1898,757 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="21.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="21.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="13.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="23"/>
+      <c r="A1" s="34"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="35"/>
     </row>
     <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22"/>
-      <c r="B2" s="24" t="s">
+      <c r="A2" s="34"/>
+      <c r="B2" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="23"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="35"/>
       <c r="M2" s="1"/>
       <c r="R2" s="2"/>
     </row>
-    <row r="3" s="28" customFormat="true" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="23"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="S3" s="29"/>
-      <c r="T3" s="29"/>
-      <c r="XFB3" s="0"/>
-      <c r="XFC3" s="0"/>
-      <c r="XFD3" s="0"/>
-    </row>
-    <row r="4" s="28" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="22"/>
-      <c r="B4" s="30" t="s">
+    <row r="3" s="40" customFormat="true" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="35"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="41"/>
+      <c r="Q3" s="41"/>
+      <c r="S3" s="41"/>
+      <c r="T3" s="41"/>
+      <c r="XFB3" s="1"/>
+      <c r="XFC3" s="1"/>
+      <c r="XFD3" s="1"/>
+    </row>
+    <row r="4" s="40" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="34"/>
+      <c r="B4" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="32" t="s">
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="33" t="s">
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="23"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29"/>
-      <c r="S4" s="29"/>
-      <c r="T4" s="29"/>
-      <c r="XFB4" s="0"/>
-      <c r="XFC4" s="0"/>
-      <c r="XFD4" s="0"/>
-    </row>
-    <row r="5" s="28" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22"/>
-      <c r="B5" s="34" t="n">
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="35"/>
+      <c r="N4" s="41"/>
+      <c r="O4" s="41"/>
+      <c r="P4" s="41"/>
+      <c r="Q4" s="41"/>
+      <c r="S4" s="41"/>
+      <c r="T4" s="41"/>
+      <c r="XFB4" s="1"/>
+      <c r="XFC4" s="1"/>
+      <c r="XFD4" s="1"/>
+    </row>
+    <row r="5" s="40" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="34"/>
+      <c r="B5" s="46" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="36"/>
-      <c r="F5" s="37" t="s">
+      <c r="E5" s="48"/>
+      <c r="F5" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="38" t="s">
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="23"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="S5" s="29"/>
-      <c r="T5" s="29"/>
-      <c r="XFB5" s="0"/>
-      <c r="XFC5" s="0"/>
-      <c r="XFD5" s="0"/>
-    </row>
-    <row r="6" s="28" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="22"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="39" t="s">
+      <c r="J5" s="50"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="35"/>
+      <c r="N5" s="41"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="41"/>
+      <c r="Q5" s="41"/>
+      <c r="S5" s="41"/>
+      <c r="T5" s="41"/>
+      <c r="XFB5" s="1"/>
+      <c r="XFC5" s="1"/>
+      <c r="XFD5" s="1"/>
+    </row>
+    <row r="6" s="40" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="34"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="40"/>
-      <c r="F6" s="39" t="s">
+      <c r="E6" s="52"/>
+      <c r="F6" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="G6" s="41"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="43" t="s">
+      <c r="G6" s="53"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
-      <c r="L6" s="23"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="S6" s="29"/>
-      <c r="T6" s="29"/>
-      <c r="XFB6" s="0"/>
-      <c r="XFC6" s="0"/>
-      <c r="XFD6" s="0"/>
-    </row>
-    <row r="7" s="28" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="22"/>
-      <c r="B7" s="44"/>
-      <c r="C7" s="39" t="s">
+      <c r="J6" s="55"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="35"/>
+      <c r="N6" s="41"/>
+      <c r="O6" s="41"/>
+      <c r="P6" s="41"/>
+      <c r="Q6" s="41"/>
+      <c r="S6" s="41"/>
+      <c r="T6" s="41"/>
+      <c r="XFB6" s="1"/>
+      <c r="XFC6" s="1"/>
+      <c r="XFD6" s="1"/>
+    </row>
+    <row r="7" s="40" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="34"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="40"/>
-      <c r="F7" s="39" t="s">
+      <c r="E7" s="52"/>
+      <c r="F7" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="G7" s="45" t="n">
+      <c r="G7" s="57" t="n">
         <v>1</v>
       </c>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39" t="s">
+      <c r="H7" s="51"/>
+      <c r="I7" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="46" t="n">
+      <c r="J7" s="58" t="n">
         <v>12000000</v>
       </c>
-      <c r="K7" s="47"/>
-      <c r="L7" s="48"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29"/>
-      <c r="S7" s="29"/>
-      <c r="T7" s="29"/>
-      <c r="XFB7" s="0"/>
-      <c r="XFC7" s="0"/>
-      <c r="XFD7" s="0"/>
-    </row>
-    <row r="8" s="28" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="22"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="39" t="s">
+      <c r="K7" s="59"/>
+      <c r="L7" s="60"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="41"/>
+      <c r="P7" s="41"/>
+      <c r="Q7" s="41"/>
+      <c r="S7" s="41"/>
+      <c r="T7" s="41"/>
+      <c r="XFB7" s="1"/>
+      <c r="XFC7" s="1"/>
+      <c r="XFD7" s="1"/>
+    </row>
+    <row r="8" s="40" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="34"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="40"/>
-      <c r="F8" s="39" t="s">
+      <c r="E8" s="52"/>
+      <c r="F8" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="G8" s="45" t="n">
+      <c r="G8" s="57" t="n">
         <v>2018</v>
       </c>
-      <c r="H8" s="42"/>
-      <c r="I8" s="39" t="s">
+      <c r="H8" s="54"/>
+      <c r="I8" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="J8" s="46" t="n">
+      <c r="J8" s="58" t="n">
         <v>1200000</v>
       </c>
-      <c r="K8" s="43"/>
-      <c r="L8" s="49"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
-      <c r="S8" s="29"/>
-      <c r="T8" s="29"/>
-      <c r="XFB8" s="0"/>
-      <c r="XFC8" s="0"/>
-      <c r="XFD8" s="0"/>
-    </row>
-    <row r="9" s="28" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="22"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="39" t="s">
+      <c r="K8" s="55"/>
+      <c r="L8" s="61"/>
+      <c r="N8" s="41"/>
+      <c r="O8" s="41"/>
+      <c r="P8" s="41"/>
+      <c r="Q8" s="41"/>
+      <c r="S8" s="41"/>
+      <c r="T8" s="41"/>
+      <c r="XFB8" s="1"/>
+      <c r="XFC8" s="1"/>
+      <c r="XFD8" s="1"/>
+    </row>
+    <row r="9" s="40" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="34"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="40" t="s">
+      <c r="D9" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="40"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39" t="s">
+      <c r="E9" s="52"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="46" t="n">
+      <c r="J9" s="58" t="n">
         <v>0</v>
       </c>
-      <c r="K9" s="47"/>
-      <c r="L9" s="49"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-      <c r="S9" s="29"/>
-      <c r="T9" s="29"/>
-      <c r="XFB9" s="0"/>
-      <c r="XFC9" s="0"/>
-      <c r="XFD9" s="0"/>
-    </row>
-    <row r="10" s="28" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="22"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="39" t="s">
+      <c r="K9" s="59"/>
+      <c r="L9" s="61"/>
+      <c r="N9" s="41"/>
+      <c r="O9" s="41"/>
+      <c r="P9" s="41"/>
+      <c r="Q9" s="41"/>
+      <c r="S9" s="41"/>
+      <c r="T9" s="41"/>
+      <c r="XFB9" s="1"/>
+      <c r="XFC9" s="1"/>
+      <c r="XFD9" s="1"/>
+    </row>
+    <row r="10" s="40" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="34"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="40"/>
-      <c r="F10" s="39" t="s">
+      <c r="E10" s="52"/>
+      <c r="F10" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="40" t="s">
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="40"/>
-      <c r="K10" s="50"/>
-      <c r="L10" s="23"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="29"/>
-      <c r="S10" s="29"/>
-      <c r="T10" s="29"/>
-      <c r="XFB10" s="0"/>
-      <c r="XFC10" s="0"/>
-      <c r="XFD10" s="0"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="62"/>
+      <c r="L10" s="35"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="41"/>
+      <c r="P10" s="41"/>
+      <c r="Q10" s="41"/>
+      <c r="S10" s="41"/>
+      <c r="T10" s="41"/>
+      <c r="XFB10" s="1"/>
+      <c r="XFC10" s="1"/>
+      <c r="XFD10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="22"/>
-      <c r="B11" s="44"/>
-      <c r="C11" s="39" t="s">
+      <c r="A11" s="34"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="51" t="s">
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="G11" s="51"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="40" t="s">
+      <c r="G11" s="63"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="40"/>
-      <c r="K11" s="50"/>
-      <c r="L11" s="23"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="62"/>
+      <c r="L11" s="35"/>
     </row>
     <row r="12" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="22"/>
-      <c r="B12" s="52"/>
-      <c r="C12" s="53" t="s">
+      <c r="A12" s="34"/>
+      <c r="B12" s="64"/>
+      <c r="C12" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="54" t="s">
+      <c r="D12" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="54"/>
-      <c r="F12" s="53" t="s">
+      <c r="E12" s="66"/>
+      <c r="F12" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="54" t="s">
+      <c r="G12" s="65"/>
+      <c r="H12" s="65"/>
+      <c r="I12" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="J12" s="54"/>
-      <c r="K12" s="55"/>
-      <c r="L12" s="23"/>
+      <c r="J12" s="66"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="35"/>
       <c r="M12" s="1"/>
       <c r="R12" s="2"/>
     </row>
-    <row r="13" s="28" customFormat="true" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="23"/>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="29"/>
-      <c r="S13" s="29"/>
-      <c r="T13" s="29"/>
-      <c r="XFB13" s="0"/>
-      <c r="XFC13" s="0"/>
-      <c r="XFD13" s="0"/>
+    <row r="13" s="40" customFormat="true" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="35"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="41"/>
+      <c r="S13" s="41"/>
+      <c r="T13" s="41"/>
+      <c r="XFB13" s="1"/>
+      <c r="XFC13" s="1"/>
+      <c r="XFD13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="32" t="s">
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="33" t="s">
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="J14" s="33"/>
-      <c r="K14" s="33"/>
+      <c r="J14" s="45"/>
+      <c r="K14" s="45"/>
     </row>
     <row r="15" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="34" t="n">
+      <c r="B15" s="46" t="n">
         <v>2</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="35" t="s">
+      <c r="D15" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="36"/>
-      <c r="F15" s="37" t="s">
+      <c r="E15" s="48"/>
+      <c r="F15" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="38" t="s">
+      <c r="G15" s="49"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="50"/>
     </row>
     <row r="16" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="34"/>
-      <c r="C16" s="39" t="s">
+      <c r="B16" s="46"/>
+      <c r="C16" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="40"/>
-      <c r="F16" s="39" t="s">
+      <c r="E16" s="52"/>
+      <c r="F16" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="G16" s="41"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="43" t="s">
+      <c r="G16" s="53"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="J16" s="43"/>
-      <c r="K16" s="43"/>
+      <c r="J16" s="55"/>
+      <c r="K16" s="55"/>
     </row>
     <row r="17" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="44"/>
-      <c r="C17" s="39" t="s">
+      <c r="B17" s="56"/>
+      <c r="C17" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="40" t="s">
+      <c r="D17" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="40"/>
-      <c r="F17" s="39" t="s">
+      <c r="E17" s="52"/>
+      <c r="F17" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="G17" s="45" t="n">
+      <c r="G17" s="57" t="n">
         <v>1</v>
       </c>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39" t="s">
+      <c r="H17" s="51"/>
+      <c r="I17" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="J17" s="46" t="n">
+      <c r="J17" s="58" t="n">
         <v>13000000</v>
       </c>
-      <c r="K17" s="47"/>
+      <c r="K17" s="59"/>
     </row>
     <row r="18" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="44"/>
-      <c r="C18" s="39" t="s">
+      <c r="B18" s="56"/>
+      <c r="C18" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="40" t="s">
+      <c r="D18" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="40"/>
-      <c r="F18" s="39" t="s">
+      <c r="E18" s="52"/>
+      <c r="F18" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="G18" s="45" t="n">
+      <c r="G18" s="57" t="n">
         <v>2018</v>
       </c>
-      <c r="H18" s="42"/>
-      <c r="I18" s="39" t="s">
+      <c r="H18" s="54"/>
+      <c r="I18" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="J18" s="46" t="n">
+      <c r="J18" s="58" t="n">
         <v>1300000</v>
       </c>
-      <c r="K18" s="43"/>
+      <c r="K18" s="55"/>
     </row>
     <row r="19" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="44"/>
-      <c r="C19" s="39" t="s">
+      <c r="B19" s="56"/>
+      <c r="C19" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="40" t="s">
+      <c r="D19" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="40"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="39" t="s">
+      <c r="E19" s="52"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="J19" s="46" t="n">
+      <c r="J19" s="58" t="n">
         <v>0</v>
       </c>
-      <c r="K19" s="47"/>
+      <c r="K19" s="59"/>
     </row>
     <row r="20" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="44"/>
-      <c r="C20" s="39" t="s">
+      <c r="B20" s="56"/>
+      <c r="C20" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="40" t="s">
+      <c r="D20" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="40"/>
-      <c r="F20" s="39" t="s">
+      <c r="E20" s="52"/>
+      <c r="F20" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="40" t="s">
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="40"/>
-      <c r="K20" s="50"/>
+      <c r="J20" s="52"/>
+      <c r="K20" s="62"/>
     </row>
     <row r="21" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="44"/>
-      <c r="C21" s="39" t="s">
+      <c r="B21" s="56"/>
+      <c r="C21" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="51" t="s">
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="G21" s="51"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="40" t="s">
+      <c r="G21" s="63"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="J21" s="40"/>
-      <c r="K21" s="50"/>
+      <c r="J21" s="52"/>
+      <c r="K21" s="62"/>
     </row>
     <row r="22" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="52"/>
-      <c r="C22" s="53" t="s">
+      <c r="B22" s="64"/>
+      <c r="C22" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="D22" s="54" t="s">
+      <c r="D22" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="E22" s="54"/>
-      <c r="F22" s="53" t="s">
+      <c r="E22" s="66"/>
+      <c r="F22" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="G22" s="53"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="54" t="s">
+      <c r="G22" s="65"/>
+      <c r="H22" s="65"/>
+      <c r="I22" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="J22" s="54"/>
-      <c r="K22" s="55"/>
+      <c r="J22" s="66"/>
+      <c r="K22" s="67"/>
     </row>
     <row r="23" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="34"/>
     </row>
     <row r="24" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="31" t="s">
+      <c r="C24" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="32" t="s">
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="33" t="s">
+      <c r="G24" s="44"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="J24" s="33"/>
-      <c r="K24" s="33"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="45"/>
     </row>
     <row r="25" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="34" t="n">
+      <c r="B25" s="46" t="n">
         <v>3</v>
       </c>
-      <c r="C25" s="35" t="s">
+      <c r="C25" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="35" t="s">
+      <c r="D25" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="E25" s="36"/>
-      <c r="F25" s="37" t="s">
+      <c r="E25" s="48"/>
+      <c r="F25" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="G25" s="37"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="38" t="s">
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="J25" s="38"/>
-      <c r="K25" s="38"/>
+      <c r="J25" s="50"/>
+      <c r="K25" s="50"/>
     </row>
     <row r="26" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="34"/>
-      <c r="C26" s="39" t="s">
+      <c r="B26" s="46"/>
+      <c r="C26" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="D26" s="40" t="s">
+      <c r="D26" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="E26" s="40"/>
-      <c r="F26" s="39" t="s">
+      <c r="E26" s="52"/>
+      <c r="F26" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="G26" s="41"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="43" t="s">
+      <c r="G26" s="53"/>
+      <c r="H26" s="54"/>
+      <c r="I26" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="J26" s="43"/>
-      <c r="K26" s="43"/>
+      <c r="J26" s="55"/>
+      <c r="K26" s="55"/>
     </row>
     <row r="27" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="44"/>
-      <c r="C27" s="39" t="s">
+      <c r="B27" s="56"/>
+      <c r="C27" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="D27" s="40" t="s">
+      <c r="D27" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="E27" s="40"/>
-      <c r="F27" s="39" t="s">
+      <c r="E27" s="52"/>
+      <c r="F27" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="G27" s="45" t="n">
+      <c r="G27" s="57" t="n">
         <v>1</v>
       </c>
-      <c r="H27" s="39"/>
-      <c r="I27" s="39" t="s">
+      <c r="H27" s="51"/>
+      <c r="I27" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="J27" s="46" t="n">
+      <c r="J27" s="58" t="n">
         <v>30300000</v>
       </c>
-      <c r="K27" s="47"/>
+      <c r="K27" s="59"/>
     </row>
     <row r="28" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="44"/>
-      <c r="C28" s="39" t="s">
+      <c r="B28" s="56"/>
+      <c r="C28" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="D28" s="40" t="s">
+      <c r="D28" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="40"/>
-      <c r="F28" s="39" t="s">
+      <c r="E28" s="52"/>
+      <c r="F28" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="G28" s="45" t="n">
+      <c r="G28" s="57" t="n">
         <v>2018</v>
       </c>
-      <c r="H28" s="42"/>
-      <c r="I28" s="39" t="s">
+      <c r="H28" s="54"/>
+      <c r="I28" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="J28" s="46" t="n">
+      <c r="J28" s="58" t="n">
         <v>3030000</v>
       </c>
-      <c r="K28" s="43"/>
+      <c r="K28" s="55"/>
     </row>
     <row r="29" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="44"/>
-      <c r="C29" s="39" t="s">
+      <c r="B29" s="56"/>
+      <c r="C29" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="D29" s="40" t="s">
+      <c r="D29" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="E29" s="40"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39" t="s">
+      <c r="E29" s="52"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="J29" s="46" t="n">
+      <c r="J29" s="58" t="n">
         <v>0</v>
       </c>
-      <c r="K29" s="47"/>
+      <c r="K29" s="59"/>
     </row>
     <row r="30" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="44"/>
-      <c r="C30" s="39" t="s">
+      <c r="B30" s="56"/>
+      <c r="C30" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="D30" s="40" t="s">
+      <c r="D30" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="E30" s="40"/>
-      <c r="F30" s="39" t="s">
+      <c r="E30" s="52"/>
+      <c r="F30" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="40" t="s">
+      <c r="G30" s="51"/>
+      <c r="H30" s="51"/>
+      <c r="I30" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="J30" s="40"/>
-      <c r="K30" s="50"/>
+      <c r="J30" s="52"/>
+      <c r="K30" s="62"/>
     </row>
     <row r="31" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="44"/>
-      <c r="C31" s="39" t="s">
+      <c r="B31" s="56"/>
+      <c r="C31" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="51" t="s">
+      <c r="D31" s="52"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="G31" s="51"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="40" t="s">
+      <c r="G31" s="63"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="J31" s="40"/>
-      <c r="K31" s="50"/>
+      <c r="J31" s="52"/>
+      <c r="K31" s="62"/>
     </row>
     <row r="32" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="52"/>
-      <c r="C32" s="53" t="s">
+      <c r="B32" s="64"/>
+      <c r="C32" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="D32" s="54" t="s">
+      <c r="D32" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="E32" s="54"/>
-      <c r="F32" s="53" t="s">
+      <c r="E32" s="66"/>
+      <c r="F32" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="G32" s="53"/>
-      <c r="H32" s="53"/>
-      <c r="I32" s="54" t="s">
+      <c r="G32" s="65"/>
+      <c r="H32" s="65"/>
+      <c r="I32" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="J32" s="54"/>
-      <c r="K32" s="55"/>
+      <c r="J32" s="66"/>
+      <c r="K32" s="67"/>
     </row>
     <row r="33" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="22"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="22"/>
-      <c r="J33" s="22"/>
-      <c r="K33" s="22"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="34"/>
+      <c r="K33" s="34"/>
     </row>
     <row r="1048502" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048503" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>